<commit_message>
export assetswap functions to excel (594/1114)
</commit_message>
<xml_diff>
--- a/UnitTests/Tests/AssetSwap.xlsx
+++ b/UnitTests/Tests/AssetSwap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="120" windowWidth="14700" windowHeight="12525"/>
+    <workbookView xWindow="75" yWindow="120" windowWidth="19485" windowHeight="12525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Function</t>
   </si>
@@ -73,12 +73,48 @@
   </si>
   <si>
     <t>qlAssetSwapPayBondCoupon</t>
+  </si>
+  <si>
+    <t>blackvol</t>
+  </si>
+  <si>
+    <t>bond</t>
+  </si>
+  <si>
+    <t>ff</t>
+  </si>
+  <si>
+    <t>ibor</t>
+  </si>
+  <si>
+    <t>sched</t>
+  </si>
+  <si>
+    <t>proc</t>
+  </si>
+  <si>
+    <t>eng</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>as01#0000</t>
+  </si>
+  <si>
+    <t>as02#0000</t>
+  </si>
+  <si>
+    <t>Payment Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -116,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -125,6 +161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,11 +464,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +478,7 @@
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -458,7 +495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -475,98 +512,256 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
       <c r="D3" s="3" t="str">
         <f>IF(ISERROR(B3),"ERROR",IF(ISERROR(C3),"FAIL",IF(B3=C3,"PASS","FAIL")))</f>
-        <v>PASS</v>
-      </c>
-      <c r="E3" t="e">
-        <f>_xll.qlAssetSwap("as01",FALSE)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>FAIL</v>
+      </c>
+      <c r="E3" t="str">
+        <f>_xll.qlAssetSwap("as01",FALSE,G3,100,G5,5,G6,"actual/360",TRUE)</f>
+        <v>as01#0000</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="str">
+        <f>_xll.qlBond(,"abc","EUR",2,"target",100,L7,L3,I3)</f>
+        <v>obj_00007#0000</v>
+      </c>
+      <c r="I3" t="str">
+        <f>_xll.qlLeg(,K4:K6,L4:L6)</f>
+        <v>obj_00006#0000</v>
+      </c>
+      <c r="L3" s="4">
+        <f>_xll.qlSettingsEvaluationDate()</f>
+        <v>42644</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
       <c r="D4" s="3" t="str">
         <f t="shared" ref="D4:D12" si="0">IF(ISERROR(B4),"ERROR",IF(ISERROR(C4),"FAIL",IF(B4=C4,"PASS","FAIL")))</f>
-        <v>PASS</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>FAIL</v>
+      </c>
+      <c r="E4" t="str">
+        <f>_xll.qlAssetSwap2("as02",TRUE,G3,100,50,1,G5,5,"actual/360",,FALSE)</f>
+        <v>as02#0000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="str">
+        <f>_xll.qlFlatForward(,2,"target",5,"actual/360","continuous","annual")</f>
+        <v>obj_00000#0000</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4">
+        <f>L3+1</f>
+        <v>42645</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
       <c r="D5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>FAIL</v>
+      </c>
+      <c r="E5" t="str">
+        <f>_xll.qlAssetSwapBondLegAnalysis(E3)</f>
+        <v>Payment Date</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="str">
+        <f>_xll.qlEuribor(,"1Y",G4)</f>
+        <v>obj_00001#0000</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5" s="4">
+        <f t="shared" ref="L5:L7" si="1">L4+1</f>
+        <v>42646</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
       <c r="D6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>FAIL</v>
+      </c>
+      <c r="E6" t="str">
+        <f>_xll.qlAssetSwapFloatingLegAnalysis(E3)</f>
+        <v>Payment Date</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="str">
+        <f>_xll.qlSchedule(,L3,L7,"1Y","target","unadjusted","unadjusted","backward",FALSE)</f>
+        <v>obj_00002#0000</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6" s="4">
+        <f t="shared" si="1"/>
+        <v>42647</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
+      <c r="B7" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="D7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>ERROR</v>
+      </c>
+      <c r="E7" t="e">
+        <f>_xll.qlAssetSwapFairSpread(E3,G10)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="str">
+        <f>_xll.qlBlackConstantVol(,L7,"target",5,"actual/360")</f>
+        <v>obj_00003#0000</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7" s="4">
+        <f t="shared" si="1"/>
+        <v>42648</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
+      <c r="B8" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="D8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>ERROR</v>
+      </c>
+      <c r="E8" t="e">
+        <f>_xll.qlAssetSwapFloatingLegBPS(E3)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="str">
+        <f>_xll.qlGeneralizedBlackScholesProcess(,G7,1,"actual/360",L7,1,1)</f>
+        <v>obj_00004#0000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
+      <c r="B9" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>ERROR</v>
+      </c>
+      <c r="E9" t="e">
+        <f>_xll.qlAssetSwapFairCleanPrice(E3)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="str">
+        <f>_xll.qlPricingEngine(,"AE",G8)</f>
+        <v>obj_00005#0000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
+      <c r="B10" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>ERROR</v>
+      </c>
+      <c r="E10" t="e">
+        <f>_xll.qlAssetSwapFairNonParRepayment(E3)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="b">
+        <f>_xll.qlInstrumentSetPricingEngine(E3,G9)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
+      <c r="B11" t="b">
+        <v>1</v>
+      </c>
       <c r="D11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>FAIL</v>
+      </c>
+      <c r="E11" t="b">
+        <f>_xll.qlAssetSwapParSwap(E3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
+      </c>
+      <c r="E12" t="b">
+        <f>_xll.qlAssetSwapPayBondCoupon(E3)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resave all unit test workbooks with calculation set to manual
</commit_message>
<xml_diff>
--- a/UnitTests/Tests/AssetSwap.xlsx
+++ b/UnitTests/Tests/AssetSwap.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\reposit\QuantLibXL\UnitTests\Tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="120" windowWidth="19485" windowHeight="12525"/>
+    <workbookView xWindow="75" yWindow="120" windowWidth="19485" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
   <definedNames>
     <definedName name="UNIT_TEST" localSheetId="0">Sheet1!$A$3:$E$12</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027" calcMode="manual"/>
 </workbook>
 </file>
 
@@ -111,7 +116,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
@@ -172,12 +177,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -219,7 +227,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -252,9 +260,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -287,6 +312,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -462,7 +504,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L12"/>
   <sheetViews>
@@ -471,7 +513,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -532,11 +574,11 @@
       </c>
       <c r="G3" t="str">
         <f>_xll.qlBond(,"abc","EUR",2,"target",100,L7,L3,I3)</f>
-        <v>obj_00007#0000</v>
+        <v>obj_00005#0000</v>
       </c>
       <c r="I3" t="str">
         <f>_xll.qlLeg(,K4:K6,L4:L6)</f>
-        <v>obj_00006#0000</v>
+        <v>obj_00004#0000</v>
       </c>
       <c r="L3" s="4">
         <f>_xll.qlSettingsEvaluationDate()</f>
@@ -683,7 +725,7 @@
       </c>
       <c r="G8" t="str">
         <f>_xll.qlGeneralizedBlackScholesProcess(,G7,1,"actual/360",L7,1,1)</f>
-        <v>obj_00004#0000</v>
+        <v>obj_00008#0000</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -706,7 +748,7 @@
       </c>
       <c r="G9" t="str">
         <f>_xll.qlPricingEngine(,"AE",G8)</f>
-        <v>obj_00005#0000</v>
+        <v>obj_00009#0000</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -771,26 +813,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>